<commit_message>
Improved comments and added conversion of dataset to lon lat coordinates
</commit_message>
<xml_diff>
--- a/config_results.xlsx
+++ b/config_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mocci\Desktop\MOST\Sardegna180\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7034C10E-4FD1-4293-B117-6FFFC31361DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FAD239-DDCF-4C2D-AD52-56AAB3235652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="610" yWindow="1010" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -150,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -158,11 +158,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -170,8 +250,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -461,7 +551,7 @@
   <dimension ref="A1:AC61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,40 +604,40 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F2">
-        <v>1.048</v>
-      </c>
-      <c r="G2">
-        <v>0.59199999999999997</v>
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.73199999999999998</v>
       </c>
       <c r="H2">
-        <v>0.84099999999999997</v>
+        <v>0.374</v>
       </c>
       <c r="I2">
-        <v>0.25700000000000001</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="J2">
-        <v>0.34599999999999997</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="K2">
-        <v>0.86299999999999999</v>
-      </c>
-      <c r="L2">
-        <v>414.1</v>
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="L2" s="5">
+        <v>576.5</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" t="s">
@@ -556,40 +646,40 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
       <c r="C3">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F3">
-        <v>1.048</v>
-      </c>
-      <c r="G3">
-        <v>0.59199999999999997</v>
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.73199999999999998</v>
       </c>
       <c r="H3">
-        <v>0.84099999999999997</v>
+        <v>0.374</v>
       </c>
       <c r="I3">
-        <v>0.25700000000000001</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="J3">
-        <v>0.34599999999999997</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="K3">
-        <v>0.86299999999999999</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="L3">
-        <v>414.9</v>
+        <v>717</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" t="s">
@@ -598,7 +688,7 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -607,31 +697,31 @@
         <v>1E-4</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F4">
-        <v>0.66500000000000004</v>
-      </c>
-      <c r="G4">
-        <v>0.71799999999999997</v>
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.73199999999999998</v>
       </c>
       <c r="H4">
-        <v>0.34799999999999998</v>
+        <v>0.374</v>
       </c>
       <c r="I4">
-        <v>0.66500000000000004</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="J4">
-        <v>0.63800000000000001</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="K4">
-        <v>0.97799999999999998</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="L4">
-        <v>416.7</v>
+        <v>761.3</v>
       </c>
       <c r="Q4" s="4"/>
       <c r="R4" t="s">
@@ -640,49 +730,49 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
       <c r="C5">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F5">
-        <v>0.91800000000000004</v>
-      </c>
-      <c r="G5">
-        <v>0.63</v>
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.73199999999999998</v>
       </c>
       <c r="H5">
-        <v>0.55900000000000005</v>
+        <v>0.374</v>
       </c>
       <c r="I5">
-        <v>0.54900000000000004</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="J5">
-        <v>0.46800000000000003</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="K5">
-        <v>0.94899999999999995</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="L5">
-        <v>419.5</v>
-      </c>
-      <c r="Q5" s="6"/>
+        <v>832.7</v>
+      </c>
+      <c r="Q5" s="5"/>
       <c r="R5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -694,53 +784,53 @@
         <v>13</v>
       </c>
       <c r="E6">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="H6">
+        <v>0.374</v>
+      </c>
+      <c r="I6">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="J6">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="K6">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="L6">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>1E-4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
         <v>32</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>0.64400000000000002</v>
       </c>
-      <c r="G6">
-        <v>0.71799999999999997</v>
-      </c>
-      <c r="H6">
-        <v>0.33100000000000002</v>
-      </c>
-      <c r="I6">
-        <v>0.67600000000000005</v>
-      </c>
-      <c r="J6">
-        <v>0.628</v>
-      </c>
-      <c r="K6">
-        <v>0.98399999999999999</v>
-      </c>
-      <c r="L6">
-        <v>428.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="5">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="5">
-        <v>32</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0.64400000000000002</v>
-      </c>
-      <c r="G7" s="5">
+      <c r="G7">
         <v>0.72099999999999997</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7">
         <v>0.34799999999999998</v>
       </c>
       <c r="I7" s="3">
@@ -749,49 +839,49 @@
       <c r="J7" s="3">
         <v>0.69099999999999995</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7">
         <v>0.97899999999999998</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="5">
         <v>429</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>5</v>
       </c>
       <c r="C8">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>32</v>
       </c>
       <c r="F8">
-        <v>0.91800000000000004</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="G8">
-        <v>0.63</v>
+        <v>0.72099999999999997</v>
       </c>
       <c r="H8">
-        <v>0.55900000000000005</v>
-      </c>
-      <c r="I8">
-        <v>0.54900000000000004</v>
-      </c>
-      <c r="J8">
-        <v>0.46800000000000003</v>
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.69099999999999995</v>
       </c>
       <c r="K8">
-        <v>0.94899999999999995</v>
-      </c>
-      <c r="L8">
-        <v>430.2</v>
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="L8" s="5">
+        <v>484.4</v>
       </c>
       <c r="R8" t="s">
         <v>24</v>
@@ -799,13 +889,13 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>5</v>
       </c>
       <c r="C9">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -814,122 +904,122 @@
         <v>32</v>
       </c>
       <c r="F9">
-        <v>0.95299999999999996</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="G9">
-        <v>0.63300000000000001</v>
+        <v>0.72099999999999997</v>
       </c>
       <c r="H9">
-        <v>0.61799999999999999</v>
-      </c>
-      <c r="I9">
-        <v>0.54200000000000004</v>
-      </c>
-      <c r="J9">
-        <v>0.46300000000000002</v>
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.69099999999999995</v>
       </c>
       <c r="K9">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="L9">
-        <v>430.6</v>
-      </c>
-      <c r="R9" s="5" t="s">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="L9" s="5">
+        <v>531.5</v>
+      </c>
+      <c r="R9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S9" s="5">
-        <v>5</v>
-      </c>
-      <c r="T9" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="U9" s="5" t="s">
+      <c r="S9" s="7">
+        <v>5</v>
+      </c>
+      <c r="T9" s="7">
+        <v>1E-4</v>
+      </c>
+      <c r="U9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V9" s="5">
+      <c r="V9" s="7">
         <v>32</v>
       </c>
-      <c r="W9" s="5">
+      <c r="W9" s="7">
         <v>0.64400000000000002</v>
       </c>
-      <c r="X9" s="5">
+      <c r="X9" s="7">
         <v>0.72099999999999997</v>
       </c>
-      <c r="Y9" s="5">
+      <c r="Y9" s="7">
         <v>0.34799999999999998</v>
       </c>
-      <c r="Z9" s="3">
+      <c r="Z9" s="8">
         <v>0.68799999999999994</v>
       </c>
-      <c r="AA9" s="3">
+      <c r="AA9" s="8">
         <v>0.69099999999999995</v>
       </c>
-      <c r="AB9" s="5">
+      <c r="AB9" s="7">
         <v>0.97899999999999998</v>
       </c>
-      <c r="AC9" s="6">
+      <c r="AC9" s="9">
         <v>429</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
       <c r="C10">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E10">
         <v>32</v>
       </c>
       <c r="F10">
-        <v>0.91800000000000004</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="G10">
-        <v>0.63</v>
+        <v>0.72099999999999997</v>
       </c>
       <c r="H10">
-        <v>0.55900000000000005</v>
-      </c>
-      <c r="I10">
-        <v>0.54900000000000004</v>
-      </c>
-      <c r="J10">
-        <v>0.46800000000000003</v>
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.69099999999999995</v>
       </c>
       <c r="K10">
-        <v>0.94899999999999995</v>
-      </c>
-      <c r="L10">
-        <v>435.4</v>
-      </c>
-      <c r="R10" s="5" t="s">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="L10" s="5">
+        <v>543.29999999999995</v>
+      </c>
+      <c r="R10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="S10" s="5">
-        <v>5</v>
-      </c>
-      <c r="T10" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="U10" s="5" t="s">
+      <c r="S10">
+        <v>5</v>
+      </c>
+      <c r="T10">
+        <v>1E-4</v>
+      </c>
+      <c r="U10" t="s">
         <v>15</v>
       </c>
-      <c r="V10" s="5">
+      <c r="V10">
         <v>32</v>
       </c>
-      <c r="W10" s="5">
+      <c r="W10">
         <v>0.64400000000000002</v>
       </c>
-      <c r="X10" s="5">
+      <c r="X10">
         <v>0.72099999999999997</v>
       </c>
-      <c r="Y10" s="5">
+      <c r="Y10">
         <v>0.34799999999999998</v>
       </c>
       <c r="Z10" s="3">
@@ -938,16 +1028,16 @@
       <c r="AA10" s="3">
         <v>0.69099999999999995</v>
       </c>
-      <c r="AB10" s="5">
+      <c r="AB10">
         <v>0.97899999999999998</v>
       </c>
-      <c r="AC10" s="6">
+      <c r="AC10" s="11">
         <v>484.4</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -956,54 +1046,54 @@
         <v>1E-4</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E11">
         <v>32</v>
       </c>
       <c r="F11">
-        <v>0.66500000000000004</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="G11">
-        <v>0.71799999999999997</v>
+        <v>0.72099999999999997</v>
       </c>
       <c r="H11">
         <v>0.34799999999999998</v>
       </c>
-      <c r="I11">
-        <v>0.66500000000000004</v>
-      </c>
-      <c r="J11">
-        <v>0.63800000000000001</v>
+      <c r="I11" s="3">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.69099999999999995</v>
       </c>
       <c r="K11">
-        <v>0.97799999999999998</v>
+        <v>0.97899999999999998</v>
       </c>
       <c r="L11">
-        <v>440.2</v>
-      </c>
-      <c r="R11" s="5" t="s">
+        <v>609.79999999999995</v>
+      </c>
+      <c r="R11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="S11" s="5">
-        <v>5</v>
-      </c>
-      <c r="T11" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="U11" s="5" t="s">
+      <c r="S11">
+        <v>5</v>
+      </c>
+      <c r="T11">
+        <v>1E-4</v>
+      </c>
+      <c r="U11" t="s">
         <v>15</v>
       </c>
-      <c r="V11" s="5">
+      <c r="V11">
         <v>32</v>
       </c>
-      <c r="W11" s="5">
+      <c r="W11">
         <v>0.64400000000000002</v>
       </c>
-      <c r="X11" s="5">
+      <c r="X11">
         <v>0.72099999999999997</v>
       </c>
-      <c r="Y11" s="5">
+      <c r="Y11">
         <v>0.34799999999999998</v>
       </c>
       <c r="Z11" s="3">
@@ -1012,16 +1102,16 @@
       <c r="AA11" s="3">
         <v>0.69099999999999995</v>
       </c>
-      <c r="AB11" s="5">
+      <c r="AB11">
         <v>0.97899999999999998</v>
       </c>
-      <c r="AC11" s="6">
+      <c r="AC11" s="11">
         <v>531.5</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -1054,30 +1144,30 @@
         <v>0.97799999999999998</v>
       </c>
       <c r="L12">
-        <v>445.2</v>
-      </c>
-      <c r="R12" s="5" t="s">
+        <v>416.7</v>
+      </c>
+      <c r="R12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="S12" s="5">
-        <v>5</v>
-      </c>
-      <c r="T12" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="U12" s="5" t="s">
+      <c r="S12">
+        <v>5</v>
+      </c>
+      <c r="T12">
+        <v>1E-4</v>
+      </c>
+      <c r="U12" t="s">
         <v>15</v>
       </c>
-      <c r="V12" s="5">
+      <c r="V12">
         <v>32</v>
       </c>
-      <c r="W12" s="5">
+      <c r="W12">
         <v>0.64400000000000002</v>
       </c>
-      <c r="X12" s="5">
+      <c r="X12">
         <v>0.72099999999999997</v>
       </c>
-      <c r="Y12" s="5">
+      <c r="Y12">
         <v>0.34799999999999998</v>
       </c>
       <c r="Z12" s="3">
@@ -1086,16 +1176,16 @@
       <c r="AA12" s="3">
         <v>0.69099999999999995</v>
       </c>
-      <c r="AB12" s="5">
+      <c r="AB12">
         <v>0.97899999999999998</v>
       </c>
-      <c r="AC12" s="6">
+      <c r="AC12" s="11">
         <v>543.29999999999995</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -1128,42 +1218,42 @@
         <v>0.98399999999999999</v>
       </c>
       <c r="L13">
-        <v>473.9</v>
-      </c>
-      <c r="R13" s="5" t="s">
+        <v>428.8</v>
+      </c>
+      <c r="R13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="S13" s="5">
-        <v>5</v>
-      </c>
-      <c r="T13" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="U13" s="5" t="s">
+      <c r="S13">
+        <v>5</v>
+      </c>
+      <c r="T13">
+        <v>1E-4</v>
+      </c>
+      <c r="U13" t="s">
         <v>13</v>
       </c>
-      <c r="V13" s="5">
-        <v>16</v>
-      </c>
-      <c r="W13" s="5">
+      <c r="V13">
+        <v>16</v>
+      </c>
+      <c r="W13">
         <v>0.70499999999999996</v>
       </c>
       <c r="X13" s="2">
         <v>0.73199999999999998</v>
       </c>
-      <c r="Y13" s="5">
+      <c r="Y13">
         <v>0.374</v>
       </c>
-      <c r="Z13" s="5">
+      <c r="Z13">
         <v>0.68300000000000005</v>
       </c>
-      <c r="AA13" s="5">
+      <c r="AA13">
         <v>0.61699999999999999</v>
       </c>
-      <c r="AB13" s="5">
+      <c r="AB13">
         <v>0.97299999999999998</v>
       </c>
-      <c r="AC13" s="6">
+      <c r="AC13" s="11">
         <v>576.5</v>
       </c>
     </row>
@@ -1175,57 +1265,57 @@
         <v>5</v>
       </c>
       <c r="C14">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14">
         <v>32</v>
       </c>
       <c r="F14">
-        <v>0.95299999999999996</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="G14">
-        <v>0.63300000000000001</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="H14">
-        <v>0.61799999999999999</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="I14">
-        <v>0.54200000000000004</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="J14">
-        <v>0.46300000000000002</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="K14">
-        <v>0.92300000000000004</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="L14">
-        <v>481.8</v>
-      </c>
-      <c r="R14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="S14" s="5">
-        <v>5</v>
-      </c>
-      <c r="T14" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="U14" s="5" t="s">
+        <v>440.2</v>
+      </c>
+      <c r="R14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="S14">
+        <v>5</v>
+      </c>
+      <c r="T14">
+        <v>1E-4</v>
+      </c>
+      <c r="U14" t="s">
         <v>15</v>
       </c>
-      <c r="V14" s="5">
+      <c r="V14">
         <v>32</v>
       </c>
-      <c r="W14" s="5">
+      <c r="W14">
         <v>0.64400000000000002</v>
       </c>
-      <c r="X14" s="5">
+      <c r="X14">
         <v>0.72099999999999997</v>
       </c>
-      <c r="Y14" s="5">
+      <c r="Y14">
         <v>0.34799999999999998</v>
       </c>
       <c r="Z14" s="3">
@@ -1234,90 +1324,90 @@
       <c r="AA14" s="3">
         <v>0.69099999999999995</v>
       </c>
-      <c r="AB14" s="5">
+      <c r="AB14">
         <v>0.97899999999999998</v>
       </c>
-      <c r="AC14" s="5">
+      <c r="AC14" s="12">
         <v>609.79999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="5">
-        <v>5</v>
-      </c>
-      <c r="C15" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D15" s="5" t="s">
+    <row r="15" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>1E-4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15">
+        <v>32</v>
+      </c>
+      <c r="F15">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="G15">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="H15">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="I15">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="J15">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="K15">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="L15">
+        <v>445.2</v>
+      </c>
+      <c r="R15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="S15" s="14">
+        <v>5</v>
+      </c>
+      <c r="T15" s="14">
+        <v>1E-4</v>
+      </c>
+      <c r="U15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="5">
-        <v>32</v>
-      </c>
-      <c r="F15" s="5">
-        <v>0.64400000000000002</v>
-      </c>
-      <c r="G15" s="5">
-        <v>0.72099999999999997</v>
-      </c>
-      <c r="H15" s="5">
-        <v>0.34799999999999998</v>
-      </c>
-      <c r="I15" s="3">
-        <v>0.68799999999999994</v>
-      </c>
-      <c r="J15" s="3">
-        <v>0.69099999999999995</v>
-      </c>
-      <c r="K15" s="5">
-        <v>0.97899999999999998</v>
-      </c>
-      <c r="L15" s="6">
-        <v>484.4</v>
-      </c>
-      <c r="R15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="S15" s="5">
-        <v>5</v>
-      </c>
-      <c r="T15" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="U15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="V15" s="5">
-        <v>16</v>
-      </c>
-      <c r="W15" s="5">
+      <c r="V15" s="14">
+        <v>16</v>
+      </c>
+      <c r="W15" s="14">
         <v>0.69799999999999995</v>
       </c>
-      <c r="X15" s="5">
+      <c r="X15" s="14">
         <v>0.70899999999999996</v>
       </c>
-      <c r="Y15" s="5">
+      <c r="Y15" s="14">
         <v>0.32400000000000001</v>
       </c>
-      <c r="Z15" s="5">
+      <c r="Z15" s="14">
         <v>0.66800000000000004</v>
       </c>
-      <c r="AA15" s="5">
+      <c r="AA15" s="14">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AB15" s="4">
+      <c r="AB15" s="15">
         <v>0.98899999999999999</v>
       </c>
-      <c r="AC15" s="5">
+      <c r="AC15" s="16">
         <v>619.79999999999995</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -1350,48 +1440,48 @@
         <v>0.98399999999999999</v>
       </c>
       <c r="L16">
-        <v>488.6</v>
-      </c>
-      <c r="R16" s="5" t="s">
+        <v>473.9</v>
+      </c>
+      <c r="R16" t="s">
         <v>18</v>
       </c>
-      <c r="S16" s="5">
-        <v>5</v>
-      </c>
-      <c r="T16" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="U16" s="5" t="s">
+      <c r="S16">
+        <v>5</v>
+      </c>
+      <c r="T16">
+        <v>1E-4</v>
+      </c>
+      <c r="U16" t="s">
         <v>13</v>
       </c>
-      <c r="V16" s="5">
-        <v>16</v>
-      </c>
-      <c r="W16" s="5">
+      <c r="V16">
+        <v>16</v>
+      </c>
+      <c r="W16">
         <v>0.70499999999999996</v>
       </c>
       <c r="X16" s="2">
         <v>0.73199999999999998</v>
       </c>
-      <c r="Y16" s="5">
+      <c r="Y16">
         <v>0.374</v>
       </c>
-      <c r="Z16" s="5">
+      <c r="Z16">
         <v>0.68300000000000005</v>
       </c>
-      <c r="AA16" s="5">
+      <c r="AA16">
         <v>0.61699999999999999</v>
       </c>
-      <c r="AB16" s="5">
+      <c r="AB16">
         <v>0.97299999999999998</v>
       </c>
-      <c r="AC16" s="5">
+      <c r="AC16">
         <v>717</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -1424,48 +1514,48 @@
         <v>0.98399999999999999</v>
       </c>
       <c r="L17">
-        <v>493.4</v>
-      </c>
-      <c r="R17" s="5" t="s">
+        <v>488.6</v>
+      </c>
+      <c r="R17" t="s">
         <v>12</v>
       </c>
-      <c r="S17" s="5">
-        <v>5</v>
-      </c>
-      <c r="T17" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="U17" s="5" t="s">
+      <c r="S17">
+        <v>5</v>
+      </c>
+      <c r="T17">
+        <v>1E-4</v>
+      </c>
+      <c r="U17" t="s">
         <v>15</v>
       </c>
-      <c r="V17" s="5">
-        <v>16</v>
-      </c>
-      <c r="W17" s="5">
+      <c r="V17">
+        <v>16</v>
+      </c>
+      <c r="W17">
         <v>0.69799999999999995</v>
       </c>
-      <c r="X17" s="5">
+      <c r="X17">
         <v>0.70899999999999996</v>
       </c>
-      <c r="Y17" s="5">
+      <c r="Y17">
         <v>0.32400000000000001</v>
       </c>
-      <c r="Z17" s="5">
+      <c r="Z17">
         <v>0.66800000000000004</v>
       </c>
-      <c r="AA17" s="5">
+      <c r="AA17">
         <v>0.57999999999999996</v>
       </c>
       <c r="AB17" s="4">
         <v>0.98899999999999999</v>
       </c>
-      <c r="AC17" s="5">
+      <c r="AC17">
         <v>730.1</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -1474,66 +1564,66 @@
         <v>1E-4</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18">
         <v>32</v>
       </c>
       <c r="F18">
-        <v>0.66500000000000004</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="G18">
         <v>0.71799999999999997</v>
       </c>
       <c r="H18">
-        <v>0.34799999999999998</v>
+        <v>0.33100000000000002</v>
       </c>
       <c r="I18">
-        <v>0.66500000000000004</v>
+        <v>0.67600000000000005</v>
       </c>
       <c r="J18">
-        <v>0.63800000000000001</v>
+        <v>0.628</v>
       </c>
       <c r="K18">
-        <v>0.97799999999999998</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="L18">
-        <v>501.9</v>
-      </c>
-      <c r="R18" s="5" t="s">
+        <v>493.4</v>
+      </c>
+      <c r="R18" t="s">
         <v>19</v>
       </c>
-      <c r="S18" s="5">
-        <v>5</v>
-      </c>
-      <c r="T18" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="U18" s="5" t="s">
+      <c r="S18">
+        <v>5</v>
+      </c>
+      <c r="T18">
+        <v>1E-4</v>
+      </c>
+      <c r="U18" t="s">
         <v>15</v>
       </c>
-      <c r="V18" s="5">
-        <v>16</v>
-      </c>
-      <c r="W18" s="5">
+      <c r="V18">
+        <v>16</v>
+      </c>
+      <c r="W18">
         <v>0.69799999999999995</v>
       </c>
-      <c r="X18" s="5">
+      <c r="X18">
         <v>0.70899999999999996</v>
       </c>
-      <c r="Y18" s="5">
+      <c r="Y18">
         <v>0.32400000000000001</v>
       </c>
-      <c r="Z18" s="5">
+      <c r="Z18">
         <v>0.66800000000000004</v>
       </c>
-      <c r="AA18" s="5">
+      <c r="AA18">
         <v>0.57999999999999996</v>
       </c>
       <c r="AB18" s="4">
         <v>0.98899999999999999</v>
       </c>
-      <c r="AC18" s="5">
+      <c r="AC18">
         <v>748.7</v>
       </c>
     </row>
@@ -1548,72 +1638,72 @@
         <v>1E-4</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E19">
         <v>32</v>
       </c>
       <c r="F19">
-        <v>0.64400000000000002</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="G19">
         <v>0.71799999999999997</v>
       </c>
       <c r="H19">
-        <v>0.33100000000000002</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="I19">
-        <v>0.67600000000000005</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="J19">
-        <v>0.628</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="K19">
-        <v>0.98399999999999999</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="L19">
-        <v>503.3</v>
-      </c>
-      <c r="R19" s="5" t="s">
+        <v>501.9</v>
+      </c>
+      <c r="R19" t="s">
         <v>19</v>
       </c>
-      <c r="S19" s="5">
-        <v>5</v>
-      </c>
-      <c r="T19" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="U19" s="5" t="s">
+      <c r="S19">
+        <v>5</v>
+      </c>
+      <c r="T19">
+        <v>1E-4</v>
+      </c>
+      <c r="U19" t="s">
         <v>13</v>
       </c>
-      <c r="V19" s="5">
-        <v>16</v>
-      </c>
-      <c r="W19" s="5">
+      <c r="V19">
+        <v>16</v>
+      </c>
+      <c r="W19">
         <v>0.70499999999999996</v>
       </c>
       <c r="X19" s="2">
         <v>0.73199999999999998</v>
       </c>
-      <c r="Y19" s="5">
+      <c r="Y19">
         <v>0.374</v>
       </c>
-      <c r="Z19" s="5">
+      <c r="Z19">
         <v>0.68300000000000005</v>
       </c>
-      <c r="AA19" s="5">
+      <c r="AA19">
         <v>0.61699999999999999</v>
       </c>
-      <c r="AB19" s="5">
+      <c r="AB19">
         <v>0.97299999999999998</v>
       </c>
-      <c r="AC19" s="5">
+      <c r="AC19">
         <v>761.3</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B20">
         <v>5</v>
@@ -1622,78 +1712,78 @@
         <v>1E-4</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <v>32</v>
       </c>
       <c r="F20">
-        <v>0.66500000000000004</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="G20">
         <v>0.71799999999999997</v>
       </c>
       <c r="H20">
-        <v>0.34799999999999998</v>
+        <v>0.33100000000000002</v>
       </c>
       <c r="I20">
-        <v>0.66500000000000004</v>
+        <v>0.67600000000000005</v>
       </c>
       <c r="J20">
-        <v>0.63800000000000001</v>
+        <v>0.628</v>
       </c>
       <c r="K20">
-        <v>0.97799999999999998</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="L20">
-        <v>505.2</v>
-      </c>
-      <c r="R20" s="5" t="s">
+        <v>503.3</v>
+      </c>
+      <c r="R20" t="s">
         <v>18</v>
       </c>
-      <c r="S20" s="5">
-        <v>5</v>
-      </c>
-      <c r="T20" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="U20" s="5" t="s">
+      <c r="S20">
+        <v>5</v>
+      </c>
+      <c r="T20">
+        <v>1E-4</v>
+      </c>
+      <c r="U20" t="s">
         <v>15</v>
       </c>
-      <c r="V20" s="5">
-        <v>16</v>
-      </c>
-      <c r="W20" s="5">
+      <c r="V20">
+        <v>16</v>
+      </c>
+      <c r="W20">
         <v>0.69799999999999995</v>
       </c>
-      <c r="X20" s="5">
+      <c r="X20">
         <v>0.70899999999999996</v>
       </c>
-      <c r="Y20" s="5">
+      <c r="Y20">
         <v>0.32400000000000001</v>
       </c>
-      <c r="Z20" s="5">
+      <c r="Z20">
         <v>0.66800000000000004</v>
       </c>
-      <c r="AA20" s="5">
+      <c r="AA20">
         <v>0.57999999999999996</v>
       </c>
       <c r="AB20" s="4">
         <v>0.98899999999999999</v>
       </c>
-      <c r="AC20" s="5">
+      <c r="AC20">
         <v>771.1</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <v>5</v>
       </c>
       <c r="C21">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D21" t="s">
         <v>14</v>
@@ -1702,366 +1792,366 @@
         <v>32</v>
       </c>
       <c r="F21">
-        <v>1.048</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="G21">
-        <v>0.59199999999999997</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="H21">
-        <v>0.84099999999999997</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="I21">
-        <v>0.25700000000000001</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="J21">
-        <v>0.34599999999999997</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="K21">
-        <v>0.86299999999999999</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="L21">
-        <v>510.7</v>
-      </c>
-      <c r="R21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="S21" s="5">
-        <v>5</v>
-      </c>
-      <c r="T21" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="U21" s="5" t="s">
+        <v>505.2</v>
+      </c>
+      <c r="R21" t="s">
+        <v>16</v>
+      </c>
+      <c r="S21">
+        <v>5</v>
+      </c>
+      <c r="T21">
+        <v>1E-4</v>
+      </c>
+      <c r="U21" t="s">
         <v>15</v>
       </c>
-      <c r="V21" s="5">
-        <v>16</v>
-      </c>
-      <c r="W21" s="5">
+      <c r="V21">
+        <v>16</v>
+      </c>
+      <c r="W21">
         <v>0.69799999999999995</v>
       </c>
-      <c r="X21" s="5">
+      <c r="X21">
         <v>0.70899999999999996</v>
       </c>
-      <c r="Y21" s="5">
+      <c r="Y21">
         <v>0.32400000000000001</v>
       </c>
-      <c r="Z21" s="5">
+      <c r="Z21">
         <v>0.66800000000000004</v>
       </c>
-      <c r="AA21" s="5">
+      <c r="AA21">
         <v>0.57999999999999996</v>
       </c>
       <c r="AB21" s="4">
         <v>0.98899999999999999</v>
       </c>
-      <c r="AC21" s="5">
+      <c r="AC21">
         <v>830.3</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22">
         <v>5</v>
       </c>
       <c r="C22">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D22" t="s">
         <v>15</v>
       </c>
       <c r="E22">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F22">
-        <v>0.95299999999999996</v>
+        <v>0.69799999999999995</v>
       </c>
       <c r="G22">
-        <v>0.63300000000000001</v>
+        <v>0.70899999999999996</v>
       </c>
       <c r="H22">
-        <v>0.61799999999999999</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="I22">
-        <v>0.54200000000000004</v>
+        <v>0.66800000000000004</v>
       </c>
       <c r="J22">
-        <v>0.46300000000000002</v>
-      </c>
-      <c r="K22">
-        <v>0.92300000000000004</v>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0.98899999999999999</v>
       </c>
       <c r="L22">
-        <v>524.9</v>
-      </c>
-      <c r="R22" s="5" t="s">
+        <v>619.79999999999995</v>
+      </c>
+      <c r="R22" t="s">
         <v>12</v>
       </c>
-      <c r="S22" s="5">
-        <v>5</v>
-      </c>
-      <c r="T22" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="U22" s="5" t="s">
+      <c r="S22">
+        <v>5</v>
+      </c>
+      <c r="T22">
+        <v>1E-4</v>
+      </c>
+      <c r="U22" t="s">
         <v>13</v>
       </c>
-      <c r="V22" s="5">
-        <v>16</v>
-      </c>
-      <c r="W22" s="5">
+      <c r="V22">
+        <v>16</v>
+      </c>
+      <c r="W22">
         <v>0.70499999999999996</v>
       </c>
       <c r="X22" s="2">
         <v>0.73199999999999998</v>
       </c>
-      <c r="Y22" s="5">
+      <c r="Y22">
         <v>0.374</v>
       </c>
-      <c r="Z22" s="5">
+      <c r="Z22">
         <v>0.68300000000000005</v>
       </c>
-      <c r="AA22" s="5">
+      <c r="AA22">
         <v>0.61699999999999999</v>
       </c>
-      <c r="AB22" s="5">
+      <c r="AB22">
         <v>0.97299999999999998</v>
       </c>
-      <c r="AC22" s="5">
+      <c r="AC22">
         <v>832.7</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="5">
-        <v>5</v>
-      </c>
-      <c r="C23" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D23" s="5" t="s">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>1E-4</v>
+      </c>
+      <c r="D23" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="5">
-        <v>32</v>
-      </c>
-      <c r="F23" s="5">
-        <v>0.64400000000000002</v>
-      </c>
-      <c r="G23" s="5">
-        <v>0.72099999999999997</v>
-      </c>
-      <c r="H23" s="5">
-        <v>0.34799999999999998</v>
-      </c>
-      <c r="I23" s="3">
-        <v>0.68799999999999994</v>
-      </c>
-      <c r="J23" s="3">
-        <v>0.69099999999999995</v>
-      </c>
-      <c r="K23" s="5">
-        <v>0.97899999999999998</v>
-      </c>
-      <c r="L23" s="6">
-        <v>531.5</v>
-      </c>
-      <c r="R23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="S23" s="5">
-        <v>5</v>
-      </c>
-      <c r="T23" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="U23" s="5" t="s">
+      <c r="E23">
+        <v>16</v>
+      </c>
+      <c r="F23">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="G23">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="H23">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="I23">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="J23">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="L23">
+        <v>730.1</v>
+      </c>
+      <c r="R23" t="s">
+        <v>16</v>
+      </c>
+      <c r="S23">
+        <v>5</v>
+      </c>
+      <c r="T23">
+        <v>1E-4</v>
+      </c>
+      <c r="U23" t="s">
         <v>13</v>
       </c>
-      <c r="V23" s="5">
-        <v>16</v>
-      </c>
-      <c r="W23" s="5">
+      <c r="V23">
+        <v>16</v>
+      </c>
+      <c r="W23">
         <v>0.70499999999999996</v>
       </c>
       <c r="X23" s="2">
         <v>0.73199999999999998</v>
       </c>
-      <c r="Y23" s="5">
+      <c r="Y23">
         <v>0.374</v>
       </c>
-      <c r="Z23" s="5">
+      <c r="Z23">
         <v>0.68300000000000005</v>
       </c>
-      <c r="AA23" s="5">
+      <c r="AA23">
         <v>0.61699999999999999</v>
       </c>
-      <c r="AB23" s="5">
+      <c r="AB23">
         <v>0.97299999999999998</v>
       </c>
-      <c r="AC23" s="5">
+      <c r="AC23">
         <v>884</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>5</v>
       </c>
       <c r="C24">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F24">
-        <v>1.048</v>
+        <v>0.69799999999999995</v>
       </c>
       <c r="G24">
-        <v>0.59199999999999997</v>
+        <v>0.70899999999999996</v>
       </c>
       <c r="H24">
-        <v>0.84099999999999997</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="I24">
-        <v>0.25700000000000001</v>
+        <v>0.66800000000000004</v>
       </c>
       <c r="J24">
-        <v>0.34599999999999997</v>
-      </c>
-      <c r="K24">
-        <v>0.86299999999999999</v>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K24" s="4">
+        <v>0.98899999999999999</v>
       </c>
       <c r="L24">
-        <v>534.9</v>
+        <v>748.7</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="5">
-        <v>5</v>
-      </c>
-      <c r="C25" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D25" s="5" t="s">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>1E-4</v>
+      </c>
+      <c r="D25" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="5">
-        <v>32</v>
-      </c>
-      <c r="F25" s="5">
-        <v>0.64400000000000002</v>
-      </c>
-      <c r="G25" s="5">
-        <v>0.72099999999999997</v>
-      </c>
-      <c r="H25" s="5">
-        <v>0.34799999999999998</v>
-      </c>
-      <c r="I25" s="3">
-        <v>0.68799999999999994</v>
-      </c>
-      <c r="J25" s="3">
-        <v>0.69099999999999995</v>
-      </c>
-      <c r="K25" s="5">
-        <v>0.97899999999999998</v>
-      </c>
-      <c r="L25" s="6">
-        <v>543.29999999999995</v>
+      <c r="E25">
+        <v>16</v>
+      </c>
+      <c r="F25">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="G25">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="H25">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="I25">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="J25">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="L25">
+        <v>771.1</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26">
         <v>5</v>
       </c>
       <c r="C26">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E26">
         <v>16</v>
       </c>
       <c r="F26">
-        <v>1.008</v>
+        <v>0.69799999999999995</v>
       </c>
       <c r="G26">
-        <v>0.61699999999999999</v>
+        <v>0.70899999999999996</v>
       </c>
       <c r="H26">
-        <v>0.755</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="I26">
-        <v>0.45800000000000002</v>
+        <v>0.66800000000000004</v>
       </c>
       <c r="J26">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="K26">
-        <v>0.88700000000000001</v>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K26" s="4">
+        <v>0.98899999999999999</v>
       </c>
       <c r="L26">
-        <v>555.79999999999995</v>
+        <v>830.3</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B27">
         <v>5</v>
       </c>
       <c r="C27">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E27">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F27">
-        <v>0.95299999999999996</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="G27">
-        <v>0.63300000000000001</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="H27">
-        <v>0.61799999999999999</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="I27">
-        <v>0.54200000000000004</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="J27">
-        <v>0.46300000000000002</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="K27">
-        <v>0.92300000000000004</v>
+        <v>0.96299999999999997</v>
       </c>
       <c r="L27">
-        <v>558.1</v>
+        <v>565.20000000000005</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B28">
         <v>5</v>
@@ -2094,126 +2184,126 @@
         <v>0.96299999999999997</v>
       </c>
       <c r="L28">
-        <v>565.20000000000005</v>
+        <v>683.1</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="5">
-        <v>5</v>
-      </c>
-      <c r="C29" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="5">
-        <v>16</v>
-      </c>
-      <c r="F29" s="5">
-        <v>0.70499999999999996</v>
-      </c>
-      <c r="G29" s="2">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="H29" s="5">
-        <v>0.374</v>
-      </c>
-      <c r="I29" s="5">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="J29" s="5">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="K29" s="5">
-        <v>0.97299999999999998</v>
-      </c>
-      <c r="L29" s="6">
-        <v>576.5</v>
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>1E-4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29">
+        <v>16</v>
+      </c>
+      <c r="F29">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="G29">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="H29">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="I29">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="J29">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="K29">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="L29">
+        <v>687.1</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30">
         <v>5</v>
       </c>
       <c r="C30">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E30">
         <v>16</v>
       </c>
       <c r="F30">
-        <v>0.999</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="G30">
-        <v>0.6</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="H30">
-        <v>0.77500000000000002</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="I30">
-        <v>0.432</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="J30">
-        <v>0.373</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="K30">
-        <v>0.875</v>
+        <v>0.96299999999999997</v>
       </c>
       <c r="L30">
-        <v>579.20000000000005</v>
+        <v>761.3</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31">
         <v>5</v>
       </c>
       <c r="C31">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E31">
         <v>16</v>
       </c>
       <c r="F31">
-        <v>1.008</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="G31">
-        <v>0.60699999999999998</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="H31">
-        <v>0.80500000000000005</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="I31">
-        <v>0.60699999999999998</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="J31">
-        <v>0.40100000000000002</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="K31">
-        <v>0.876</v>
+        <v>0.96299999999999997</v>
       </c>
       <c r="L31">
-        <v>585.20000000000005</v>
+        <v>863.3</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B32">
         <v>5</v>
@@ -2222,31 +2312,31 @@
         <v>1E-3</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E32">
         <v>32</v>
       </c>
       <c r="F32">
-        <v>0.91800000000000004</v>
+        <v>0.95299999999999996</v>
       </c>
       <c r="G32">
-        <v>0.63</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="H32">
-        <v>0.55900000000000005</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="I32">
-        <v>0.54900000000000004</v>
+        <v>0.54200000000000004</v>
       </c>
       <c r="J32">
-        <v>0.46800000000000003</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="K32">
-        <v>0.94899999999999995</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="L32">
-        <v>594.29999999999995</v>
+        <v>430.6</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
@@ -2260,36 +2350,36 @@
         <v>1E-3</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E33">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F33">
-        <v>1.008</v>
+        <v>0.95299999999999996</v>
       </c>
       <c r="G33">
-        <v>0.61699999999999999</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="H33">
-        <v>0.755</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="I33">
-        <v>0.45800000000000002</v>
+        <v>0.54200000000000004</v>
       </c>
       <c r="J33">
-        <v>0.39800000000000002</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="K33">
-        <v>0.88700000000000001</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="L33">
-        <v>599</v>
+        <v>481.8</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -2298,74 +2388,74 @@
         <v>1E-3</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E34">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F34">
-        <v>1.008</v>
+        <v>0.95299999999999996</v>
       </c>
       <c r="G34">
-        <v>0.61699999999999999</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="H34">
-        <v>0.755</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="I34">
-        <v>0.45800000000000002</v>
+        <v>0.54200000000000004</v>
       </c>
       <c r="J34">
-        <v>0.39800000000000002</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="K34">
-        <v>0.88700000000000001</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="L34">
-        <v>603.6</v>
+        <v>524.9</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="5">
-        <v>5</v>
-      </c>
-      <c r="C35" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D35" s="5" t="s">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>1E-3</v>
+      </c>
+      <c r="D35" t="s">
         <v>15</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35">
         <v>32</v>
       </c>
-      <c r="F35" s="5">
-        <v>0.64400000000000002</v>
-      </c>
-      <c r="G35" s="5">
-        <v>0.72099999999999997</v>
-      </c>
-      <c r="H35" s="5">
-        <v>0.34799999999999998</v>
-      </c>
-      <c r="I35" s="3">
-        <v>0.68799999999999994</v>
-      </c>
-      <c r="J35" s="3">
-        <v>0.69099999999999995</v>
-      </c>
-      <c r="K35" s="5">
-        <v>0.97899999999999998</v>
-      </c>
-      <c r="L35" s="5">
-        <v>609.79999999999995</v>
+      <c r="F35">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="G35">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="H35">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="I35">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="J35">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="K35">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="L35">
+        <v>558.1</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B36">
         <v>5</v>
@@ -2377,71 +2467,71 @@
         <v>15</v>
       </c>
       <c r="E36">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F36">
-        <v>0.97399999999999998</v>
+        <v>0.95299999999999996</v>
       </c>
       <c r="G36">
-        <v>0.61399999999999999</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="H36">
-        <v>0.75</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="I36">
-        <v>0.433</v>
+        <v>0.54200000000000004</v>
       </c>
       <c r="J36">
-        <v>0.41299999999999998</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="K36">
-        <v>0.89</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="L36">
-        <v>614.1</v>
+        <v>787.2</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="5">
-        <v>5</v>
-      </c>
-      <c r="C37" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="5">
-        <v>16</v>
-      </c>
-      <c r="F37" s="5">
-        <v>0.69799999999999995</v>
-      </c>
-      <c r="G37" s="5">
-        <v>0.70899999999999996</v>
-      </c>
-      <c r="H37" s="5">
-        <v>0.32400000000000001</v>
-      </c>
-      <c r="I37" s="5">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="J37" s="5">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="K37" s="4">
-        <v>0.98899999999999999</v>
-      </c>
-      <c r="L37" s="5">
-        <v>619.79999999999995</v>
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>1E-3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37">
+        <v>32</v>
+      </c>
+      <c r="F37">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="G37">
+        <v>0.63</v>
+      </c>
+      <c r="H37">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="I37">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="J37">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="K37">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="L37">
+        <v>419.5</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38">
         <v>5</v>
@@ -2474,7 +2564,7 @@
         <v>0.94899999999999995</v>
       </c>
       <c r="L38">
-        <v>622.6</v>
+        <v>430.2</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
@@ -2488,31 +2578,31 @@
         <v>1E-3</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E39">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F39">
-        <v>0.97399999999999998</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="G39">
-        <v>0.61399999999999999</v>
+        <v>0.63</v>
       </c>
       <c r="H39">
-        <v>0.75</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="I39">
-        <v>0.433</v>
+        <v>0.54900000000000004</v>
       </c>
       <c r="J39">
-        <v>0.41299999999999998</v>
+        <v>0.46800000000000003</v>
       </c>
       <c r="K39">
-        <v>0.89</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="L39">
-        <v>624.4</v>
+        <v>435.4</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
@@ -2526,36 +2616,36 @@
         <v>1E-3</v>
       </c>
       <c r="D40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E40">
         <v>32</v>
       </c>
       <c r="F40">
-        <v>1.048</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="G40">
-        <v>0.59199999999999997</v>
+        <v>0.63</v>
       </c>
       <c r="H40">
-        <v>0.84099999999999997</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="I40">
-        <v>0.25700000000000001</v>
+        <v>0.54900000000000004</v>
       </c>
       <c r="J40">
-        <v>0.34599999999999997</v>
+        <v>0.46800000000000003</v>
       </c>
       <c r="K40">
-        <v>0.86299999999999999</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="L40">
-        <v>624.4</v>
+        <v>594.29999999999995</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B41">
         <v>5</v>
@@ -2567,39 +2657,39 @@
         <v>13</v>
       </c>
       <c r="E41">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F41">
-        <v>1.1080000000000001</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="G41">
-        <v>0.56999999999999995</v>
+        <v>0.63</v>
       </c>
       <c r="H41">
-        <v>0.98399999999999999</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="I41">
-        <v>0.245</v>
+        <v>0.54900000000000004</v>
       </c>
       <c r="J41">
-        <v>0.32800000000000001</v>
+        <v>0.46800000000000003</v>
       </c>
       <c r="K41">
-        <v>0.83799999999999997</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="L41">
-        <v>658.3</v>
+        <v>622.6</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B42">
         <v>5</v>
       </c>
       <c r="C42">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="D42" t="s">
         <v>14</v>
@@ -2608,36 +2698,36 @@
         <v>16</v>
       </c>
       <c r="F42">
-        <v>0.70599999999999996</v>
+        <v>1.008</v>
       </c>
       <c r="G42">
-        <v>0.70199999999999996</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="H42">
-        <v>0.40899999999999997</v>
+        <v>0.755</v>
       </c>
       <c r="I42">
-        <v>0.67800000000000005</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="J42">
-        <v>0.58799999999999997</v>
+        <v>0.39800000000000002</v>
       </c>
       <c r="K42">
-        <v>0.96299999999999997</v>
+        <v>0.88700000000000001</v>
       </c>
       <c r="L42">
-        <v>683.1</v>
+        <v>555.79999999999995</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B43">
         <v>5</v>
       </c>
       <c r="C43">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="D43" t="s">
         <v>14</v>
@@ -2646,25 +2736,25 @@
         <v>16</v>
       </c>
       <c r="F43">
-        <v>0.70599999999999996</v>
+        <v>1.008</v>
       </c>
       <c r="G43">
-        <v>0.70199999999999996</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="H43">
-        <v>0.40899999999999997</v>
+        <v>0.755</v>
       </c>
       <c r="I43">
-        <v>0.67800000000000005</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="J43">
-        <v>0.58799999999999997</v>
+        <v>0.39800000000000002</v>
       </c>
       <c r="K43">
-        <v>0.96299999999999997</v>
+        <v>0.88700000000000001</v>
       </c>
       <c r="L43">
-        <v>687.1</v>
+        <v>599</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
@@ -2678,74 +2768,74 @@
         <v>1E-3</v>
       </c>
       <c r="D44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E44">
         <v>16</v>
       </c>
       <c r="F44">
-        <v>0.97399999999999998</v>
+        <v>1.008</v>
       </c>
       <c r="G44">
-        <v>0.61399999999999999</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="H44">
-        <v>0.75</v>
+        <v>0.755</v>
       </c>
       <c r="I44">
-        <v>0.433</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="J44">
-        <v>0.41299999999999998</v>
+        <v>0.39800000000000002</v>
       </c>
       <c r="K44">
-        <v>0.89</v>
+        <v>0.88700000000000001</v>
       </c>
       <c r="L44">
-        <v>691</v>
+        <v>603.6</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A45" s="5" t="s">
+      <c r="A45" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="5">
-        <v>5</v>
-      </c>
-      <c r="C45" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E45" s="5">
-        <v>16</v>
-      </c>
-      <c r="F45" s="5">
-        <v>0.70499999999999996</v>
-      </c>
-      <c r="G45" s="2">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="H45" s="5">
-        <v>0.374</v>
-      </c>
-      <c r="I45" s="5">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="J45" s="5">
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>1E-3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45">
+        <v>16</v>
+      </c>
+      <c r="F45">
+        <v>1.008</v>
+      </c>
+      <c r="G45">
         <v>0.61699999999999999</v>
       </c>
-      <c r="K45" s="5">
-        <v>0.97299999999999998</v>
-      </c>
-      <c r="L45" s="5">
-        <v>717</v>
+      <c r="H45">
+        <v>0.755</v>
+      </c>
+      <c r="I45">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="J45">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="K45">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="L45">
+        <v>723.8</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B46">
         <v>5</v>
@@ -2778,202 +2868,202 @@
         <v>0.88700000000000001</v>
       </c>
       <c r="L46">
-        <v>723.8</v>
+        <v>828.9</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A47" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B47" s="5">
-        <v>5</v>
-      </c>
-      <c r="C47" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D47" s="5" t="s">
+      <c r="A47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <v>1E-3</v>
+      </c>
+      <c r="D47" t="s">
         <v>15</v>
       </c>
-      <c r="E47" s="5">
-        <v>16</v>
-      </c>
-      <c r="F47" s="5">
-        <v>0.69799999999999995</v>
-      </c>
-      <c r="G47" s="5">
-        <v>0.70899999999999996</v>
-      </c>
-      <c r="H47" s="5">
-        <v>0.32400000000000001</v>
-      </c>
-      <c r="I47" s="5">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="J47" s="5">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="K47" s="4">
-        <v>0.98899999999999999</v>
-      </c>
-      <c r="L47" s="5">
-        <v>730.1</v>
+      <c r="E47">
+        <v>16</v>
+      </c>
+      <c r="F47">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="G47">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="H47">
+        <v>0.75</v>
+      </c>
+      <c r="I47">
+        <v>0.433</v>
+      </c>
+      <c r="J47">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="K47">
+        <v>0.89</v>
+      </c>
+      <c r="L47">
+        <v>614.1</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A48" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" s="5">
-        <v>5</v>
-      </c>
-      <c r="C48" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D48" s="5" t="s">
+      <c r="A48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <v>1E-3</v>
+      </c>
+      <c r="D48" t="s">
         <v>15</v>
       </c>
-      <c r="E48" s="5">
-        <v>16</v>
-      </c>
-      <c r="F48" s="5">
-        <v>0.69799999999999995</v>
-      </c>
-      <c r="G48" s="5">
-        <v>0.70899999999999996</v>
-      </c>
-      <c r="H48" s="5">
-        <v>0.32400000000000001</v>
-      </c>
-      <c r="I48" s="5">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="J48" s="5">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="K48" s="4">
-        <v>0.98899999999999999</v>
-      </c>
-      <c r="L48" s="5">
-        <v>748.7</v>
+      <c r="E48">
+        <v>16</v>
+      </c>
+      <c r="F48">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="G48">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="H48">
+        <v>0.75</v>
+      </c>
+      <c r="I48">
+        <v>0.433</v>
+      </c>
+      <c r="J48">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="K48">
+        <v>0.89</v>
+      </c>
+      <c r="L48">
+        <v>624.4</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A49" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" s="5">
-        <v>5</v>
-      </c>
-      <c r="C49" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E49" s="5">
-        <v>16</v>
-      </c>
-      <c r="F49" s="5">
-        <v>0.70499999999999996</v>
-      </c>
-      <c r="G49" s="2">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="H49" s="5">
-        <v>0.374</v>
-      </c>
-      <c r="I49" s="5">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="J49" s="5">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="K49" s="5">
-        <v>0.97299999999999998</v>
-      </c>
-      <c r="L49" s="5">
-        <v>761.3</v>
+      <c r="A49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>1E-3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49">
+        <v>16</v>
+      </c>
+      <c r="F49">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="G49">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="H49">
+        <v>0.75</v>
+      </c>
+      <c r="I49">
+        <v>0.433</v>
+      </c>
+      <c r="J49">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="K49">
+        <v>0.89</v>
+      </c>
+      <c r="L49">
+        <v>691</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B50">
         <v>5</v>
       </c>
       <c r="C50">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="D50" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E50">
         <v>16</v>
       </c>
       <c r="F50">
-        <v>0.70599999999999996</v>
+        <v>0.97399999999999998</v>
       </c>
       <c r="G50">
-        <v>0.70199999999999996</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="H50">
-        <v>0.40899999999999997</v>
+        <v>0.75</v>
       </c>
       <c r="I50">
-        <v>0.67800000000000005</v>
+        <v>0.433</v>
       </c>
       <c r="J50">
-        <v>0.58799999999999997</v>
+        <v>0.41299999999999998</v>
       </c>
       <c r="K50">
-        <v>0.96299999999999997</v>
+        <v>0.89</v>
       </c>
       <c r="L50">
-        <v>761.3</v>
+        <v>824.9</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A51" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" s="5">
-        <v>5</v>
-      </c>
-      <c r="C51" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D51" s="5" t="s">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51">
+        <v>1E-3</v>
+      </c>
+      <c r="D51" t="s">
         <v>15</v>
       </c>
-      <c r="E51" s="5">
-        <v>16</v>
-      </c>
-      <c r="F51" s="5">
-        <v>0.69799999999999995</v>
-      </c>
-      <c r="G51" s="5">
-        <v>0.70899999999999996</v>
-      </c>
-      <c r="H51" s="5">
-        <v>0.32400000000000001</v>
-      </c>
-      <c r="I51" s="5">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="J51" s="5">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="K51" s="4">
-        <v>0.98899999999999999</v>
-      </c>
-      <c r="L51" s="5">
-        <v>771.1</v>
+      <c r="E51">
+        <v>16</v>
+      </c>
+      <c r="F51">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="G51">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="H51">
+        <v>0.75</v>
+      </c>
+      <c r="I51">
+        <v>0.433</v>
+      </c>
+      <c r="J51">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="K51">
+        <v>0.89</v>
+      </c>
+      <c r="L51">
+        <v>837.8</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B52">
         <v>5</v>
@@ -2982,36 +3072,36 @@
         <v>1E-3</v>
       </c>
       <c r="D52" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E52">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F52">
-        <v>0.95299999999999996</v>
+        <v>1.008</v>
       </c>
       <c r="G52">
-        <v>0.63300000000000001</v>
+        <v>0.60699999999999998</v>
       </c>
       <c r="H52">
-        <v>0.61799999999999999</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="I52">
-        <v>0.54200000000000004</v>
+        <v>0.60699999999999998</v>
       </c>
       <c r="J52">
-        <v>0.46300000000000002</v>
+        <v>0.40100000000000002</v>
       </c>
       <c r="K52">
-        <v>0.92300000000000004</v>
+        <v>0.876</v>
       </c>
       <c r="L52">
-        <v>787.2</v>
+        <v>585.20000000000005</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B53">
         <v>5</v>
@@ -3026,30 +3116,30 @@
         <v>16</v>
       </c>
       <c r="F53">
-        <v>1.022</v>
+        <v>0.999</v>
       </c>
       <c r="G53">
-        <v>0.58699999999999997</v>
+        <v>0.6</v>
       </c>
       <c r="H53">
-        <v>0.80800000000000005</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="I53">
-        <v>0.374</v>
+        <v>0.432</v>
       </c>
       <c r="J53">
-        <v>0.379</v>
+        <v>0.373</v>
       </c>
       <c r="K53">
-        <v>0.878</v>
+        <v>0.875</v>
       </c>
       <c r="L53">
-        <v>800.5</v>
+        <v>579.20000000000005</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B54">
         <v>5</v>
@@ -3058,36 +3148,36 @@
         <v>1E-3</v>
       </c>
       <c r="D54" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E54">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F54">
-        <v>0.97399999999999998</v>
+        <v>1.048</v>
       </c>
       <c r="G54">
-        <v>0.61399999999999999</v>
+        <v>0.59199999999999997</v>
       </c>
       <c r="H54">
-        <v>0.75</v>
+        <v>0.84099999999999997</v>
       </c>
       <c r="I54">
-        <v>0.433</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="J54">
-        <v>0.41299999999999998</v>
+        <v>0.34599999999999997</v>
       </c>
       <c r="K54">
-        <v>0.89</v>
+        <v>0.86299999999999999</v>
       </c>
       <c r="L54">
-        <v>824.9</v>
+        <v>414.1</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B55">
         <v>5</v>
@@ -3096,36 +3186,36 @@
         <v>1E-3</v>
       </c>
       <c r="D55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E55">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F55">
-        <v>1.091</v>
+        <v>1.048</v>
       </c>
       <c r="G55">
-        <v>0.58199999999999996</v>
+        <v>0.59199999999999997</v>
       </c>
       <c r="H55">
-        <v>0.96299999999999997</v>
+        <v>0.84099999999999997</v>
       </c>
       <c r="I55">
-        <v>0.35799999999999998</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="J55">
-        <v>0.36799999999999999</v>
+        <v>0.34599999999999997</v>
       </c>
       <c r="K55">
-        <v>0.84599999999999997</v>
+        <v>0.86299999999999999</v>
       </c>
       <c r="L55">
-        <v>828.4</v>
+        <v>414.9</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B56">
         <v>5</v>
@@ -3137,109 +3227,109 @@
         <v>14</v>
       </c>
       <c r="E56">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F56">
-        <v>1.008</v>
+        <v>1.048</v>
       </c>
       <c r="G56">
-        <v>0.61699999999999999</v>
+        <v>0.59199999999999997</v>
       </c>
       <c r="H56">
-        <v>0.755</v>
+        <v>0.84099999999999997</v>
       </c>
       <c r="I56">
-        <v>0.45800000000000002</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="J56">
-        <v>0.39800000000000002</v>
+        <v>0.34599999999999997</v>
       </c>
       <c r="K56">
-        <v>0.88700000000000001</v>
+        <v>0.86299999999999999</v>
       </c>
       <c r="L56">
-        <v>828.9</v>
+        <v>510.7</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A57" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B57" s="5">
-        <v>5</v>
-      </c>
-      <c r="C57" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E57" s="5">
-        <v>16</v>
-      </c>
-      <c r="F57" s="5">
-        <v>0.69799999999999995</v>
-      </c>
-      <c r="G57" s="5">
-        <v>0.70899999999999996</v>
-      </c>
-      <c r="H57" s="5">
-        <v>0.32400000000000001</v>
-      </c>
-      <c r="I57" s="5">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="J57" s="5">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="K57" s="4">
-        <v>0.98899999999999999</v>
-      </c>
-      <c r="L57" s="5">
-        <v>830.3</v>
+      <c r="A57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="C57">
+        <v>1E-3</v>
+      </c>
+      <c r="D57" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57">
+        <v>32</v>
+      </c>
+      <c r="F57">
+        <v>1.048</v>
+      </c>
+      <c r="G57">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="H57">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="I57">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="J57">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="K57">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="L57">
+        <v>534.9</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A58" s="5" t="s">
+      <c r="A58" t="s">
         <v>12</v>
       </c>
-      <c r="B58" s="5">
-        <v>5</v>
-      </c>
-      <c r="C58" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E58" s="5">
-        <v>16</v>
-      </c>
-      <c r="F58" s="5">
-        <v>0.70499999999999996</v>
-      </c>
-      <c r="G58" s="2">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="H58" s="5">
-        <v>0.374</v>
-      </c>
-      <c r="I58" s="5">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="J58" s="5">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="K58" s="5">
-        <v>0.97299999999999998</v>
-      </c>
-      <c r="L58" s="5">
-        <v>832.7</v>
+      <c r="B58">
+        <v>5</v>
+      </c>
+      <c r="C58">
+        <v>1E-3</v>
+      </c>
+      <c r="D58" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58">
+        <v>32</v>
+      </c>
+      <c r="F58">
+        <v>1.048</v>
+      </c>
+      <c r="G58">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="H58">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="I58">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="J58">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="K58">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="L58">
+        <v>624.4</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B59">
         <v>5</v>
@@ -3248,112 +3338,112 @@
         <v>1E-3</v>
       </c>
       <c r="D59" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E59">
         <v>16</v>
       </c>
       <c r="F59">
-        <v>0.97399999999999998</v>
+        <v>1.022</v>
       </c>
       <c r="G59">
-        <v>0.61399999999999999</v>
+        <v>0.58699999999999997</v>
       </c>
       <c r="H59">
-        <v>0.75</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="I59">
-        <v>0.433</v>
+        <v>0.374</v>
       </c>
       <c r="J59">
-        <v>0.41299999999999998</v>
+        <v>0.379</v>
       </c>
       <c r="K59">
-        <v>0.89</v>
+        <v>0.878</v>
       </c>
       <c r="L59">
-        <v>837.8</v>
+        <v>800.5</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B60">
         <v>5</v>
       </c>
       <c r="C60">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="D60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E60">
         <v>16</v>
       </c>
       <c r="F60">
-        <v>0.70599999999999996</v>
+        <v>1.091</v>
       </c>
       <c r="G60">
-        <v>0.70199999999999996</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="H60">
-        <v>0.40899999999999997</v>
+        <v>0.96299999999999997</v>
       </c>
       <c r="I60">
-        <v>0.67800000000000005</v>
+        <v>0.35799999999999998</v>
       </c>
       <c r="J60">
-        <v>0.58799999999999997</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="K60">
-        <v>0.96299999999999997</v>
+        <v>0.84599999999999997</v>
       </c>
       <c r="L60">
-        <v>863.3</v>
+        <v>828.4</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A61" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B61" s="5">
-        <v>5</v>
-      </c>
-      <c r="C61" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="D61" s="5" t="s">
+      <c r="A61" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61">
+        <v>1E-3</v>
+      </c>
+      <c r="D61" t="s">
         <v>13</v>
       </c>
-      <c r="E61" s="5">
-        <v>16</v>
-      </c>
-      <c r="F61" s="5">
-        <v>0.70499999999999996</v>
-      </c>
-      <c r="G61" s="2">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="H61" s="5">
-        <v>0.374</v>
-      </c>
-      <c r="I61" s="5">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="J61" s="5">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="K61" s="5">
-        <v>0.97299999999999998</v>
-      </c>
-      <c r="L61" s="5">
-        <v>884</v>
+      <c r="E61">
+        <v>16</v>
+      </c>
+      <c r="F61">
+        <v>1.1080000000000001</v>
+      </c>
+      <c r="G61">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H61">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="I61">
+        <v>0.245</v>
+      </c>
+      <c r="J61">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="K61">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="L61">
+        <v>658.3</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L68">
-    <sortCondition ref="L1:L68"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L61">
+    <sortCondition descending="1" ref="G1:G61"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>